<commit_message>
added phlu page types
</commit_message>
<xml_diff>
--- a/NeosNodesDefinitions.xlsx
+++ b/NeosNodesDefinitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Nodetype</t>
   </si>
@@ -59,9 +59,6 @@
     <t>TYPO3.Neos:ContentCollection</t>
   </si>
   <si>
-    <t>Childnodes</t>
-  </si>
-  <si>
     <t>Constraints</t>
   </si>
   <si>
@@ -131,7 +128,34 @@
     <t>PHLU.Corporate:Content</t>
   </si>
   <si>
-    <t>docs hinzufügen!!</t>
+    <t>docs.phlu.ch hinzufügen!!</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Overview</t>
+  </si>
+  <si>
+    <t>Childnodes (autocreated collections)</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:Overview.Onepage</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:Overview.Tiles</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:View.Detail</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:View.Dossier</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:Overview.Onepage, PHLU.Corporate:Page:View.Detail</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page:View.Detail, PHLU.Corporate:Page:View.Dossier</t>
+  </si>
+  <si>
+    <t>PHLU.Corporate:Page.Service</t>
   </si>
 </sst>
 </file>
@@ -455,20 +479,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="59.83203125" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" customWidth="1"/>
+    <col min="6" max="6" width="67.83203125" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -486,10 +510,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -498,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -506,7 +530,7 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -515,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -526,7 +550,7 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -535,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -546,16 +570,16 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -566,7 +590,7 @@
         <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -575,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -586,19 +610,19 @@
         <v>300</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -609,19 +633,19 @@
         <v>301</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>28</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -632,19 +656,19 @@
         <v>302</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -655,19 +679,19 @@
         <v>303</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -675,19 +699,19 @@
         <v>304</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -695,16 +719,16 @@
         <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -715,16 +739,19 @@
         <v>401</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -735,16 +762,16 @@
         <v>402</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -755,16 +782,16 @@
         <v>403</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -775,16 +802,16 @@
         <v>404</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -795,24 +822,133 @@
         <v>405</v>
       </c>
       <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>406</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>407</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>408</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>409</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>500</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>